<commit_message>
+++ Updated tests target source files +++ Added Performance analisys for BinaryTrees test
</commit_message>
<xml_diff>
--- a/doc/AlterNative DOCS/Performance/PT002.xlsx
+++ b/doc/AlterNative DOCS/Performance/PT002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="28515" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fannkuch-redux" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
   <si>
     <t>LINUX</t>
   </si>
@@ -123,6 +123,9 @@
   <si>
     <t>AVERAGE</t>
   </si>
+  <si>
+    <t>maxims</t>
+  </si>
 </sst>
 </file>
 
@@ -404,24 +407,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="88148992"/>
-        <c:axId val="88167168"/>
+        <c:axId val="88144512"/>
+        <c:axId val="90001792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88148992"/>
+        <c:axId val="88144512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88167168"/>
+        <c:crossAx val="90001792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88167168"/>
+        <c:axId val="90001792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,7 +432,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88148992"/>
+        <c:crossAx val="88144512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -442,13 +445,539 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Target vs Language</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$E$76</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C# ORIGINAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$75:$H$75</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>WIN32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LINUX</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ANDROID</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$76:$H$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.91265520826961899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$E$77</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++ ORIGINAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$75:$H$75</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>WIN32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LINUX</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ANDROID</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$77:$H$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30735048705708851</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22215180848872765</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$E$78</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++ ALTERNATIVE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$75:$H$75</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>WIN32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LINUX</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ANDROID</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$78:$H$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.8670458947540115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35118077385803548</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2417813970436794</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="44205952"/>
+        <c:axId val="44374656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="44205952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Target</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44374656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="44374656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44205952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Language vs Target</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WIN32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$E$82:$E$84</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>C# ORIGINAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C++ ORIGINAL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C++ ALTERNATIVE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$F$82:$F$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.0918423929403188E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34978605049208389</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27865801716794442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$G$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LINUX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$E$82:$E$84</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>C# ORIGINAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C++ ORIGINAL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C++ ALTERNATIVE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$G$82:$G$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.32658312077187535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45183283411781489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47435292575846932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$H$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ANDROID</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$E$82:$E$84</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>C# ORIGINAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>C++ ORIGINAL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>C++ ALTERNATIVE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fannkuch-redux-opt-Array_nos'!$H$82:$H$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="104289792"/>
+        <c:axId val="104449152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="104289792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Language</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="104449152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="104449152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="104289792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-ES"/>
   <c:chart>
@@ -589,24 +1118,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97402880"/>
-        <c:axId val="97404416"/>
+        <c:axId val="91767552"/>
+        <c:axId val="91769088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97402880"/>
+        <c:axId val="91767552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97404416"/>
+        <c:crossAx val="91769088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97404416"/>
+        <c:axId val="91769088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +1161,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97402880"/>
+        <c:crossAx val="91767552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -645,13 +1174,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-ES"/>
   <c:chart>
@@ -792,24 +1321,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97414144"/>
-        <c:axId val="97432320"/>
+        <c:axId val="91803648"/>
+        <c:axId val="91805184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97414144"/>
+        <c:axId val="91803648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97432320"/>
+        <c:crossAx val="91805184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97432320"/>
+        <c:axId val="91805184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +1364,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97414144"/>
+        <c:crossAx val="91803648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -848,13 +1377,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-ES"/>
   <c:chart>
@@ -995,24 +1524,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97793920"/>
-        <c:axId val="97795456"/>
+        <c:axId val="91831296"/>
+        <c:axId val="91853568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97793920"/>
+        <c:axId val="91831296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97795456"/>
+        <c:crossAx val="91853568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97795456"/>
+        <c:axId val="91853568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,7 +1567,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97793920"/>
+        <c:crossAx val="91831296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1051,13 +1580,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-ES"/>
   <c:chart>
@@ -1246,11 +1775,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48968832"/>
-        <c:axId val="48970752"/>
+        <c:axId val="91894528"/>
+        <c:axId val="91896448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48968832"/>
+        <c:axId val="91894528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,14 +1803,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48970752"/>
+        <c:crossAx val="91896448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48970752"/>
+        <c:axId val="91896448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1307,7 +1836,7 @@
         </c:title>
         <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48968832"/>
+        <c:crossAx val="91894528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1318,10 +1847,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.87478122319293994"/>
-          <c:y val="0.42545234536527327"/>
-          <c:w val="0.1189630264630554"/>
-          <c:h val="0.18186652368868503"/>
+          <c:x val="0.84621950965520865"/>
+          <c:y val="0.27859419340755293"/>
+          <c:w val="0.14752477445170206"/>
+          <c:h val="0.21783182003221296"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1337,6 +1866,227 @@
           <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global comparison'!$K$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average C#</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global comparison'!$L$44:$N$44</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>DEBUG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RELEASE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global comparison'!$L$45:$N$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global comparison'!$K$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average C++ alternative</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global comparison'!$L$44:$N$44</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>DEBUG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RELEASE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global comparison'!$L$46:$N$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.82749567424587533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30328799021413938</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59024143707781862</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Global comparison'!$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average C++ original</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Global comparison'!$L$44:$N$44</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>DEBUG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>RELEASE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Global comparison'!$L$47:$N$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.46854431578098837</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28639173598128986</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38610280894120186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="43387136"/>
+        <c:axId val="43419904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43387136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43419904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43419904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43387136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1657,24 +2407,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="88207360"/>
-        <c:axId val="88208896"/>
+        <c:axId val="90037632"/>
+        <c:axId val="90571904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88207360"/>
+        <c:axId val="90037632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88208896"/>
+        <c:crossAx val="90571904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88208896"/>
+        <c:axId val="90571904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,7 +2432,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88207360"/>
+        <c:crossAx val="90037632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1695,7 +2445,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2010,24 +2760,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="89445120"/>
-        <c:axId val="89446656"/>
+        <c:axId val="90624384"/>
+        <c:axId val="90625920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89445120"/>
+        <c:axId val="90624384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89446656"/>
+        <c:crossAx val="90625920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89446656"/>
+        <c:axId val="90625920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2035,7 +2785,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89445120"/>
+        <c:crossAx val="90624384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2048,7 +2798,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2249,24 +2999,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91463040"/>
-        <c:axId val="91481216"/>
+        <c:axId val="90938368"/>
+        <c:axId val="90952448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91463040"/>
+        <c:axId val="90938368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91481216"/>
+        <c:crossAx val="90952448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91481216"/>
+        <c:axId val="90952448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2274,7 +3024,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91463040"/>
+        <c:crossAx val="90938368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2287,7 +3037,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2602,24 +3352,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="96686464"/>
-        <c:axId val="96688000"/>
+        <c:axId val="91115520"/>
+        <c:axId val="91117056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96686464"/>
+        <c:axId val="91115520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96688000"/>
+        <c:crossAx val="91117056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96688000"/>
+        <c:axId val="91117056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2627,7 +3377,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96686464"/>
+        <c:crossAx val="91115520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2640,7 +3390,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2955,24 +3705,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="96748672"/>
-        <c:axId val="96750208"/>
+        <c:axId val="91042560"/>
+        <c:axId val="91044096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96748672"/>
+        <c:axId val="91042560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96750208"/>
+        <c:crossAx val="91044096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96750208"/>
+        <c:axId val="91044096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2980,7 +3730,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96748672"/>
+        <c:crossAx val="91042560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2993,7 +3743,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3003,6 +3753,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-ES"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Compilation vs language</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3153,7 +3921,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3212,32 +3980,68 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97131904"/>
-        <c:axId val="97174656"/>
+        <c:axId val="91163648"/>
+        <c:axId val="91202304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97131904"/>
+        <c:axId val="91163648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Compilation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97174656"/>
+        <c:crossAx val="91202304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97174656"/>
+        <c:axId val="91202304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97131904"/>
+        <c:crossAx val="91163648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3250,7 +4054,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3309,7 +4113,7 @@
                   <c:v>C++ ORIGINAL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3359,7 +4163,7 @@
                   <c:v>C++ ORIGINAL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3409,7 +4213,7 @@
                   <c:v>C++ ORIGINAL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3459,7 +4263,7 @@
                   <c:v>C++ ORIGINAL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3509,7 +4313,7 @@
                   <c:v>C++ ORIGINAL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3559,7 +4363,7 @@
                   <c:v>C++ ORIGINAL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>C++ TRANSLATED</c:v>
+                  <c:v>C++ ALTERNATIVE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3583,24 +4387,42 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97214848"/>
-        <c:axId val="97216384"/>
+        <c:axId val="91586560"/>
+        <c:axId val="91588096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97214848"/>
+        <c:axId val="91586560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Language</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97216384"/>
+        <c:crossAx val="91588096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97216384"/>
+        <c:axId val="91588096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3624,9 +4446,9 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97214848"/>
+        <c:crossAx val="91586560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3639,7 +4461,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3763,7 +4585,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++ TRANSLATED D</c:v>
+                  <c:v>C++ ALTERNATIVE D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3913,7 +4735,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++ TRANSLATED R</c:v>
+                  <c:v>C++ ALTERNATIVE R</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3954,24 +4776,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="97264768"/>
-        <c:axId val="97266304"/>
+        <c:axId val="91498368"/>
+        <c:axId val="91499904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97264768"/>
+        <c:axId val="91498368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97266304"/>
+        <c:crossAx val="91499904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97266304"/>
+        <c:axId val="91499904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3979,7 +4801,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97264768"/>
+        <c:crossAx val="91498368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3992,7 +4814,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4192,16 +5014,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>529318</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>277821</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>127904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>437029</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>42182</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>194574</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>137427</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4222,16 +5044,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>331644</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>64484</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>149678</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>165797</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>72330</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4252,16 +5074,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>397087</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>500996</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>155841</xdr:rowOff>
+      <xdr:rowOff>103887</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>649940</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>424804</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>127266</xdr:rowOff>
+      <xdr:rowOff>75312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4275,6 +5097,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>107251</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>188148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>24864</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="4 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>617765</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>127908</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>745672</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>167368</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="5 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4379,14 +5261,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>672354</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>89646</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>81644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>549089</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4400,6 +5282,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="6 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4695,7 +5607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -5393,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O95" sqref="O95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5404,7 +6316,7 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
@@ -5486,7 +6398,7 @@
         <v>7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="M5" s="2">
         <f>D8</f>
@@ -5589,7 +6501,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2">
         <v>269569</v>
@@ -5615,7 +6527,7 @@
         <v>152610</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="M8" s="2">
         <f>H8</f>
@@ -5642,7 +6554,7 @@
       </c>
       <c r="F12" s="1" t="str">
         <f>C8</f>
-        <v>C++ TRANSLATED</v>
+        <v>C++ ALTERNATIVE</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -5717,7 +6629,7 @@
         <v>72391</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
+    <row r="17" spans="3:8">
       <c r="C17" s="1" t="str">
         <f>F5</f>
         <v>ANDROID DEBUG</v>
@@ -5735,7 +6647,7 @@
         <v>323370</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
+    <row r="18" spans="3:8">
       <c r="C18" s="1" t="str">
         <f>J5</f>
         <v>ANDROID RELEASE</v>
@@ -5751,6 +6663,207 @@
       <c r="F18" s="2">
         <f>J8</f>
         <v>152610</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8">
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f>M2</f>
+        <v>WIN32</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f t="shared" ref="G23:H23" si="2">N2</f>
+        <v>LINUX</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>ANDROID</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
+      <c r="E24" s="1" t="str">
+        <f>C6</f>
+        <v>C# ORIGINAL</v>
+      </c>
+      <c r="F24" s="2">
+        <f>M6</f>
+        <v>44763</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" ref="G24:H26" si="3">N6</f>
+        <v>206136</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="3"/>
+        <v>631190</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8">
+      <c r="E25" s="1" t="str">
+        <f>C7</f>
+        <v>C++ ORIGINAL</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:F26" si="4">M7</f>
+        <v>49047</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="3"/>
+        <v>63356</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="3"/>
+        <v>140220</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8">
+      <c r="E26" s="1" t="str">
+        <f>C8</f>
+        <v>C++ ALTERNATIVE</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="4"/>
+        <v>42526</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="3"/>
+        <v>72391</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="3"/>
+        <v>152610</v>
+      </c>
+    </row>
+    <row r="75" spans="5:8">
+      <c r="E75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
+        <v>0</v>
+      </c>
+      <c r="H75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="5:8">
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76">
+        <f>F24/MAX(F$24:F$26)</f>
+        <v>0.91265520826961899</v>
+      </c>
+      <c r="G76">
+        <f t="shared" ref="G76:H76" si="5">G24/MAX(G$24:G$26)</f>
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="5:8">
+      <c r="E77" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77">
+        <f t="shared" ref="F77:H78" si="6">F25/MAX(F$24:F$26)</f>
+        <v>1</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="6"/>
+        <v>0.30735048705708851</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="6"/>
+        <v>0.22215180848872765</v>
+      </c>
+    </row>
+    <row r="78" spans="5:8">
+      <c r="E78" t="s">
+        <v>27</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="6"/>
+        <v>0.8670458947540115</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="6"/>
+        <v>0.35118077385803548</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="6"/>
+        <v>0.2417813970436794</v>
+      </c>
+    </row>
+    <row r="81" spans="5:8">
+      <c r="E81" t="s">
+        <v>25</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
+        <v>0</v>
+      </c>
+      <c r="H81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="5:8">
+      <c r="E82" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82">
+        <f>F24/MAX($F24:$H24)</f>
+        <v>7.0918423929403188E-2</v>
+      </c>
+      <c r="G82">
+        <f t="shared" ref="G82:H82" si="7">G24/MAX($F24:$H24)</f>
+        <v>0.32658312077187535</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="5:8">
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83">
+        <f t="shared" ref="F83:H84" si="8">F25/MAX($F25:$H25)</f>
+        <v>0.34978605049208389</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="8"/>
+        <v>0.45183283411781489</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="5:8">
+      <c r="E84" t="s">
+        <v>27</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="8"/>
+        <v>0.27865801716794442</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="8"/>
+        <v>0.47435292575846932</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="8"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5762,10 +6875,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3:K47"/>
+  <dimension ref="C3:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5778,6 +6891,7 @@
     <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11">
@@ -5973,10 +7087,10 @@
         <v>84207.666666666672</v>
       </c>
     </row>
-    <row r="40" spans="6:10">
+    <row r="40" spans="6:14">
       <c r="J40" s="4"/>
     </row>
-    <row r="44" spans="6:10">
+    <row r="44" spans="6:14">
       <c r="F44" t="s">
         <v>33</v>
       </c>
@@ -5989,8 +7103,20 @@
       <c r="I44" t="s">
         <v>34</v>
       </c>
+      <c r="K44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L44" t="s">
+        <v>24</v>
+      </c>
+      <c r="M44" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="45" spans="6:10">
+    <row r="45" spans="6:14">
       <c r="F45" t="s">
         <v>22</v>
       </c>
@@ -6006,8 +7132,23 @@
         <f>F4</f>
         <v>324825.83333333331</v>
       </c>
+      <c r="K45" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45">
+        <f>G45/$G49</f>
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <f>H45/$H49</f>
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <f>I45/$I49</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="6:10">
+    <row r="46" spans="6:14">
       <c r="F46" t="s">
         <v>30</v>
       </c>
@@ -6023,8 +7164,23 @@
         <f>F5</f>
         <v>191725.66666666666</v>
       </c>
+      <c r="K46" t="s">
+        <v>30</v>
+      </c>
+      <c r="L46">
+        <f>G46/$G49</f>
+        <v>0.82749567424587533</v>
+      </c>
+      <c r="M46">
+        <f>H46/$H49</f>
+        <v>0.30328799021413938</v>
+      </c>
+      <c r="N46">
+        <f>I46/$I49</f>
+        <v>0.59024143707781862</v>
+      </c>
     </row>
-    <row r="47" spans="6:10">
+    <row r="47" spans="6:14">
       <c r="F47" t="s">
         <v>23</v>
       </c>
@@ -6039,6 +7195,38 @@
       <c r="I47">
         <f>F6</f>
         <v>125416.16666666667</v>
+      </c>
+      <c r="K47" t="s">
+        <v>23</v>
+      </c>
+      <c r="L47">
+        <f>G47/$G49</f>
+        <v>0.46854431578098837</v>
+      </c>
+      <c r="M47">
+        <f>H47/$H49</f>
+        <v>0.28639173598128986</v>
+      </c>
+      <c r="N47">
+        <f>I47/$I49</f>
+        <v>0.38610280894120186</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9">
+      <c r="F49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49">
+        <f>MAX(G45:G47)</f>
+        <v>355622</v>
+      </c>
+      <c r="H49">
+        <f>MAX(H45:H47)</f>
+        <v>294029.66666666669</v>
+      </c>
+      <c r="I49">
+        <f>MAX(I45:I47)</f>
+        <v>324825.83333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>